<commit_message>
Rocket Launcher Level 2 và 3. Xóa Particle Template vì nó nặng vãi lồn
Rocket Launcher Level 2 và 3. Xóa Particle Template vì nó nặng vãi lồn
</commit_message>
<xml_diff>
--- a/Thông số quái và trụ.xlsx
+++ b/Thông số quái và trụ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Project Game\Tower-Defense-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Tower Defense 1\GitHub2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E625A595-B917-45F0-9FFB-4F1FCD5D1DB8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Virus" sheetId="3" r:id="rId3"/>
     <sheet name="Beam Blaster" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -111,12 +112,24 @@
   </si>
   <si>
     <t>STT</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Animation Rate</t>
+  </si>
+  <si>
+    <t>Energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,7 +658,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -683,7 +702,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -721,7 +746,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -748,55 +779,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
-  <autoFilter ref="J8:M9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+  <autoFilter ref="J8:M9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="STT" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="Name" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" name="Assets Folder" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STT" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assets Folder" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
-  <autoFilter ref="P8:S9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+  <autoFilter ref="P8:S9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="STT" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="Name" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" name="Assets Folder" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="STT" dataDxfId="21" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Assets Folder" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="D7:G10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5D941EB8-2D8A-4E64-9CA7-DADD24AA5CE9}" name="Table3" displayName="Table3" ref="H8:K10" totalsRowShown="0">
+  <autoFilter ref="H8:K10" xr:uid="{7859AB58-8CF5-4770-89FE-7351A2A75015}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Level" dataDxfId="12" dataCellStyle="Heading 1"/>
-    <tableColumn id="2" name="Left" dataDxfId="11" dataCellStyle="Input"/>
-    <tableColumn id="3" name="Top" dataDxfId="10" dataCellStyle="Input"/>
-    <tableColumn id="4" name="Right" dataDxfId="9" dataCellStyle="Input"/>
+    <tableColumn id="1" xr3:uid="{EE9C34B5-47CE-47FD-9EFC-EE648D0320FE}" name="Health"/>
+    <tableColumn id="2" xr3:uid="{3D38B8D9-4B34-43E2-860C-225B8B7B1C2F}" name="Speed"/>
+    <tableColumn id="3" xr3:uid="{B01DA130-D3F0-4E84-AB8C-154923EE7DEC}" name="Animation Rate"/>
+    <tableColumn id="4" xr3:uid="{74CE7050-A46B-470C-9415-D84695650E5C}" name="Energy"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="K7:Q14" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="K7:Q13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="D7:G10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Level" dataDxfId="12" dataCellStyle="Heading 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Left" dataDxfId="11" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Top" dataDxfId="10" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Right" dataDxfId="9" dataCellStyle="Input"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table43" displayName="Table43" ref="K7:Q14" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="K7:Q13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Level" totalsRowLabel="Total" dataDxfId="6"/>
-    <tableColumn id="2" name="Scale" dataDxfId="5"/>
-    <tableColumn id="3" name="Fire Rate" dataDxfId="4"/>
-    <tableColumn id="4" name="Rotation Speed" dataDxfId="3"/>
-    <tableColumn id="5" name="Projectile Speed" dataDxfId="2"/>
-    <tableColumn id="7" name="Range" totalsRowFunction="count" dataDxfId="1"/>
-    <tableColumn id="8" name="Damage" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Level" totalsRowLabel="Total" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Scale" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Fire Rate" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Rotation Speed" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Projectile Speed" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Range" totalsRowFunction="count" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Damage" totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1064,7 +1108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="J6:V15"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1221,8 +1265,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K9" location="'Beam Blaster'!A1" display="Beam Blaster"/>
-    <hyperlink ref="Q9" location="Virus!A1" display="Virus"/>
+    <hyperlink ref="K9" location="'Beam Blaster'!A1" display="Beam Blaster" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q9" location="Virus!A1" display="Virus" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1234,10 +1278,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1246,23 +1292,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="H8:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>600</v>
+      </c>
+      <c r="J9">
+        <v>2.5</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D5:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Thêm và sửa 2 cái excel note thông số. Ngoài ra trong UE thì chỉnh LevelStartInitial với cả Wave Database
</commit_message>
<xml_diff>
--- a/Thông số quái và trụ.xlsx
+++ b/Thông số quái và trụ.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\Tower Defense (DOM)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Tower Defense 1\GitHub2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3565A8FC-88ED-4972-9C40-B7913D7808D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="3975" yWindow="1380" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin" sheetId="1" r:id="rId1"/>
-    <sheet name="Shocker" sheetId="4" r:id="rId2"/>
-    <sheet name="Virus" sheetId="3" r:id="rId3"/>
-    <sheet name="Beam Blaster" sheetId="2" r:id="rId4"/>
+    <sheet name="Beam Blaster" sheetId="2" r:id="rId2"/>
+    <sheet name="Shocker" sheetId="4" r:id="rId3"/>
+    <sheet name="Virus" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +42,6 @@
   </si>
   <si>
     <t>Virus</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>Fire Rate</t>
@@ -128,7 +131,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -316,7 +319,10 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="37">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -646,13 +652,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>53660</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -690,13 +696,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>44482</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -734,13 +740,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>285751</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>178542</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -778,70 +784,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="35" dataDxfId="34" totalsRowDxfId="33" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
-  <autoFilter ref="J8:M9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+  <autoFilter ref="J8:M9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="STT" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="Name" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" name="Assets Folder" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STT" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assets Folder" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
-  <autoFilter ref="P8:S9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+  <autoFilter ref="P8:S9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" name="STT" dataDxfId="21" dataCellStyle="Normal"/>
-    <tableColumn id="1" name="Name" dataDxfId="20" totalsRowDxfId="19" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" name="Assets Folder" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="STT" dataDxfId="22" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Assets Folder" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="H8:K10" totalsRowShown="0">
-  <autoFilter ref="H8:K10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="D7:G10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Health"/>
-    <tableColumn id="2" name="Speed"/>
-    <tableColumn id="3" name="Animation Rate"/>
-    <tableColumn id="4" name="Energy"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Level" dataDxfId="13" dataCellStyle="Heading 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Left" dataDxfId="12" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Top" dataDxfId="11" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Right" dataDxfId="10" dataCellStyle="Input"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="D7:G10"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Level" dataDxfId="12" dataCellStyle="Heading 1"/>
-    <tableColumn id="2" name="Left" dataDxfId="11" dataCellStyle="Input"/>
-    <tableColumn id="3" name="Top" dataDxfId="10" dataCellStyle="Input"/>
-    <tableColumn id="4" name="Right" dataDxfId="9" dataCellStyle="Input"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table43" displayName="Table43" ref="K7:R10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="K7:R10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Level" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Scale" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Fire Rate" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rotation Speed" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Projectile Speed" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Range" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Damage" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{91948A94-CC43-4FE3-A382-0FF58E507DD1}" name="Energy" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="K7:Q14" totalsRowCount="1" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="K7:Q13"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Level" totalsRowLabel="Total" dataDxfId="6"/>
-    <tableColumn id="2" name="Scale" dataDxfId="5"/>
-    <tableColumn id="3" name="Fire Rate" dataDxfId="4"/>
-    <tableColumn id="4" name="Rotation Speed" dataDxfId="3"/>
-    <tableColumn id="5" name="Projectile Speed" dataDxfId="2"/>
-    <tableColumn id="7" name="Range" totalsRowFunction="count" dataDxfId="1"/>
-    <tableColumn id="8" name="Damage" totalsRowFunction="count" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="H8:K10" totalsRowShown="0">
+  <autoFilter ref="H8:K10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Health"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Speed"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Animation Rate"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Energy"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1107,10 +1114,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="J6:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -1132,38 +1139,38 @@
   <sheetData>
     <row r="6" spans="10:22" ht="33.75" x14ac:dyDescent="0.5">
       <c r="K6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="1"/>
       <c r="Q6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="10:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="15" t="s">
         <v>0</v>
       </c>
       <c r="L8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N8" s="4"/>
       <c r="P8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q8" s="15" t="s">
         <v>0</v>
       </c>
       <c r="R8" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
@@ -1174,13 +1181,13 @@
         <v>1</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" s="4"/>
       <c r="P9" s="12">
@@ -1190,10 +1197,10 @@
         <v>2</v>
       </c>
       <c r="R9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="S9" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -1264,8 +1271,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K9" location="'Beam Blaster'!A1" display="Beam Blaster"/>
-    <hyperlink ref="Q9" location="Virus!A1" display="Virus"/>
+    <hyperlink ref="K9" location="'Beam Blaster'!A1" display="Beam Blaster" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="Q9" location="Virus!A1" display="Virus" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1277,7 +1284,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="D5:R17"/>
+  <sheetViews>
+    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:18" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="4:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <v>10</v>
+      </c>
+      <c r="O8" s="4">
+        <v>45</v>
+      </c>
+      <c r="P8" s="4">
+        <v>800</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="7">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
+        <v>12</v>
+      </c>
+      <c r="K9" s="4">
+        <v>2</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <v>10</v>
+      </c>
+      <c r="O9" s="4">
+        <v>45</v>
+      </c>
+      <c r="P9" s="4">
+        <v>900</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6">
+        <v>7</v>
+      </c>
+      <c r="G10" s="6">
+        <v>12</v>
+      </c>
+      <c r="K10" s="4">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <v>10</v>
+      </c>
+      <c r="O10" s="4">
+        <v>45</v>
+      </c>
+      <c r="P10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="4:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:16" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1290,8 +1483,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="H8:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1308,16 +1501,16 @@
   <sheetData>
     <row r="8" spans="8:11" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>30</v>
-      </c>
-      <c r="K8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="8:11" x14ac:dyDescent="0.25">
@@ -1340,222 +1533,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:Q21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="4:17" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="4:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="4:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6">
-        <v>7</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="K8" s="4">
-        <v>1</v>
-      </c>
-      <c r="L8" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="M8" s="4">
-        <v>1</v>
-      </c>
-      <c r="N8" s="4">
-        <v>10</v>
-      </c>
-      <c r="O8" s="4">
-        <v>45</v>
-      </c>
-      <c r="P8" s="4">
-        <v>800</v>
-      </c>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="4:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="7">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6">
-        <v>7</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6">
-        <v>12</v>
-      </c>
-      <c r="K9" s="4">
-        <v>2</v>
-      </c>
-      <c r="L9" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="M9" s="4">
-        <v>1</v>
-      </c>
-      <c r="N9" s="4">
-        <v>10</v>
-      </c>
-      <c r="O9" s="4">
-        <v>45</v>
-      </c>
-      <c r="P9" s="4">
-        <v>900</v>
-      </c>
-      <c r="Q9" s="4"/>
-    </row>
-    <row r="10" spans="4:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="7">
-        <v>3</v>
-      </c>
-      <c r="E10" s="6">
-        <v>21</v>
-      </c>
-      <c r="F10" s="6">
-        <v>7</v>
-      </c>
-      <c r="G10" s="6">
-        <v>12</v>
-      </c>
-      <c r="K10" s="4">
-        <v>3</v>
-      </c>
-      <c r="L10" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="M10" s="4">
-        <v>1</v>
-      </c>
-      <c r="N10" s="4">
-        <v>10</v>
-      </c>
-      <c r="O10" s="4">
-        <v>45</v>
-      </c>
-      <c r="P10" s="4">
-        <v>1000</v>
-      </c>
-      <c r="Q10" s="4"/>
-    </row>
-    <row r="11" spans="4:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-    </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-    </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="K14" t="s">
-        <v>3</v>
-      </c>
-      <c r="P14">
-        <f>SUBTOTAL(103,Table43[Range])</f>
-        <v>3</v>
-      </c>
-      <c r="Q14">
-        <f>SUBTOTAL(103,Table43[Damage])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="5:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="E21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L21" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P21" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="2">
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Chỉnh thông số chòi và quái nhưng chưa hoàn thiện
</commit_message>
<xml_diff>
--- a/Thông số quái và trụ.xlsx
+++ b/Thông số quái và trụ.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Tower Defense 1\GitHub2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3565A8FC-88ED-4972-9C40-B7913D7808D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872DA540-4661-49AC-9E1C-FE8B3C98E9A5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1380" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="2445" windowWidth="19965" windowHeight="11835" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thông tin" sheetId="1" r:id="rId1"/>
     <sheet name="Beam Blaster" sheetId="2" r:id="rId2"/>
     <sheet name="Shocker" sheetId="4" r:id="rId3"/>
-    <sheet name="Virus" sheetId="3" r:id="rId4"/>
+    <sheet name="Roclet Launcher" sheetId="7" r:id="rId4"/>
+    <sheet name="Virus" sheetId="3" r:id="rId5"/>
+    <sheet name="Worm" sheetId="5" r:id="rId6"/>
+    <sheet name="Junkmail" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -119,20 +122,23 @@
     <t>Health</t>
   </si>
   <si>
-    <t>Speed</t>
-  </si>
-  <si>
     <t>Animation Rate</t>
   </si>
   <si>
     <t>Energy</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Animation Max</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,8 +210,16 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +236,20 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -264,6 +290,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -272,7 +335,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -311,6 +374,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9"/>
@@ -319,7 +388,67 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="57">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -657,7 +786,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>53660</xdr:colOff>
+      <xdr:colOff>72710</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -701,7 +830,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>44482</xdr:rowOff>
     </xdr:to>
@@ -745,7 +874,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>178542</xdr:rowOff>
     </xdr:to>
@@ -784,69 +913,104 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="J8:M9" headerRowDxfId="56" dataDxfId="55" totalsRowDxfId="54" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
   <autoFilter ref="J8:M9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STT" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total" dataDxfId="31" totalsRowDxfId="30" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assets Folder" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="STT" dataDxfId="53" totalsRowDxfId="52" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" totalsRowLabel="Total" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Assets Folder" dataDxfId="49" totalsRowDxfId="48" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="47" totalsRowDxfId="46" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="25" dataDxfId="24" totalsRowDxfId="23" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table57" displayName="Table57" ref="P8:S9" headerRowDxfId="45" dataDxfId="44" totalsRowDxfId="43" headerRowCellStyle="Heading 3" dataCellStyle="Normal">
   <autoFilter ref="P8:S9" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="STT" dataDxfId="22" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Followed Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Assets Folder" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="STT" dataDxfId="42" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name" dataDxfId="41" totalsRowDxfId="40" dataCellStyle="Followed Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Assets Folder" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Blueprint Folder" totalsRowFunction="count" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="D7:G10" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="D7:G10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Level" dataDxfId="13" dataCellStyle="Heading 1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Left" dataDxfId="12" dataCellStyle="Input"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Top" dataDxfId="11" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Right" dataDxfId="10" dataCellStyle="Input"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Level" dataDxfId="33" dataCellStyle="Heading 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Left" dataDxfId="32" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Top" dataDxfId="31" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Right" dataDxfId="30" dataCellStyle="Input"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table43" displayName="Table43" ref="K7:R10" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table43" displayName="Table43" ref="K7:R10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="K7:R10" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Level" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Scale" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Fire Rate" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rotation Speed" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Projectile Speed" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Range" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Damage" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{91948A94-CC43-4FE3-A382-0FF58E507DD1}" name="Energy" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Level" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Scale" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Fire Rate" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Rotation Speed" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Projectile Speed" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Range" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Damage" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{91948A94-CC43-4FE3-A382-0FF58E507DD1}" name="Energy" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="H8:K10" totalsRowShown="0">
-  <autoFilter ref="H8:K10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{48B9E389-9CEA-48CC-A259-F64296D609EB}" name="Table438" displayName="Table438" ref="D4:K7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="D4:K7" xr:uid="{DF00BF45-EA9B-4505-99DC-AC3C6A57581C}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{BB197833-D77E-4ADC-909F-296C8806A303}" name="Level" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{14E4C033-B929-4BBB-8687-7336E1494AB7}" name="Scale" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{AAC5B3E1-E0FA-441E-A3AC-CE6C0EB2D735}" name="Fire Rate" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{77E6CA07-9476-499A-916B-D16A5914E2A8}" name="Rotation Speed" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{A76651CB-D3E8-454A-8C3F-EB5AF073DD3F}" name="Projectile Speed" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{4226B1C9-D05D-4790-BB10-1268D03BFF87}" name="Range" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{C1D0D693-70FD-4229-B3C3-9951D29915EA}" name="Damage" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{1D513C6A-BEBB-4A68-97B6-4E4581D65E98}" name="Energy" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{04CA26F2-5E50-44C9-BB68-AA75BB2FA856}" name="Table4310" displayName="Table4310" ref="D3:K6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="D3:K6" xr:uid="{83BB03FA-5773-4C93-92D6-6D37A3EDB7AE}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{8B7AE79F-773D-4999-8E88-EB08CFD0377C}" name="Level" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7875C1E8-F5AF-4B2C-99B7-EB199953881C}" name="Scale" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F39A132F-9971-45CF-B530-8B53F7D6494A}" name="Fire Rate" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{6BE340CE-EE6D-450B-B3F7-B4C682CEAFE5}" name="Rotation Speed" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{55E1AA4A-2DAA-4A39-B46D-6FDC3F6661FE}" name="Projectile Speed" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{108B9BCF-CEE1-4095-8125-04C9211DA789}" name="Range" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{B142C642-BDB7-40DF-97BD-C9B8E6521E9C}" name="Damage" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B38DC56C-0CC2-43E7-AB19-0D1E65CE40D2}" name="Energy" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="H8:L10" totalsRowShown="0">
+  <autoFilter ref="H8:L10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Health"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Speed"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Animation Rate"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Energy"/>
+    <tableColumn id="5" xr3:uid="{D0463527-9698-4A1B-922E-298FC80BDEF6}" name="Score"/>
+    <tableColumn id="6" xr3:uid="{716D897B-EE19-4070-B5FA-630A7B9C59EB}" name="Animation Max"/>
+    <tableColumn id="7" xr3:uid="{746741A0-E83C-4A49-9164-177935DEAC61}" name="Animation Rate"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1117,7 +1281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="J6:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -1287,20 +1451,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="D5:R17"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1347,7 +1515,7 @@
         <v>14</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1377,8 +1545,12 @@
       <c r="P8" s="4">
         <v>800</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="Q8" s="4">
+        <v>10</v>
+      </c>
+      <c r="R8" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="7">
@@ -1409,7 +1581,9 @@
       <c r="P9" s="4">
         <v>900</v>
       </c>
-      <c r="Q9" s="4"/>
+      <c r="Q9" s="4">
+        <v>10</v>
+      </c>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="4:18" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1443,7 +1617,9 @@
       <c r="P10" s="4">
         <v>1000</v>
       </c>
-      <c r="Q10" s="4"/>
+      <c r="Q10" s="4">
+        <v>10</v>
+      </c>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="4:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1471,61 +1647,128 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="D2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="H8:K9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="J5" sqref="J5:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H8" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="s">
+    <row r="2" spans="4:11" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="8:11" x14ac:dyDescent="0.25">
-      <c r="H9">
-        <v>100</v>
-      </c>
-      <c r="I9">
-        <v>600</v>
-      </c>
-      <c r="J9">
-        <v>2.5</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>45</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>45</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1533,4 +1776,266 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1012EBF-5775-4E6D-9CA3-F9D268383B21}">
+  <dimension ref="D1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="4:11" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="H8:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>300</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{011ABFF1-A489-4DAE-B427-7142428FBE19}">
+  <dimension ref="H10:L11"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="19">
+        <v>100</v>
+      </c>
+      <c r="I11" s="20">
+        <v>20</v>
+      </c>
+      <c r="J11" s="20">
+        <v>50</v>
+      </c>
+      <c r="K11" s="20">
+        <v>150</v>
+      </c>
+      <c r="L11" s="21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC964E6-7FC1-4FF9-AE2E-1AB4C2B447C4}">
+  <dimension ref="H10:L11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="10" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="19">
+        <v>25</v>
+      </c>
+      <c r="I11" s="20">
+        <v>15</v>
+      </c>
+      <c r="J11" s="20">
+        <v>25</v>
+      </c>
+      <c r="K11" s="20">
+        <v>700</v>
+      </c>
+      <c r="L11" s="21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>